<commit_message>
update species biomass file - not finisched yet
</commit_message>
<xml_diff>
--- a/Data/4. Visual census/Biomass_Species.xlsx
+++ b/Data/4. Visual census/Biomass_Species.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents/Post-Doc/Projets/Villefranche/Projets/BenthFun – Jeremy/BenthFun/Data/4. Visual census/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SZNHP213\OneDrive\Desktop\SZN\Jeremy project\Data\4. Visual census\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB2BD82-121B-D04C-B585-A6C56B74E745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16040" xr2:uid="{D1CF2BFA-78D8-1149-8471-3A76F2C50420}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="33">
   <si>
     <t>Tile</t>
   </si>
@@ -107,12 +106,36 @@
   </si>
   <si>
     <t>Ambient</t>
+  </si>
+  <si>
+    <t>Padina</t>
+  </si>
+  <si>
+    <t>Jania</t>
+  </si>
+  <si>
+    <t>Flabellia</t>
+  </si>
+  <si>
+    <t>Jania+Halopteris</t>
+  </si>
+  <si>
+    <t>Acetabularia parvula</t>
+  </si>
+  <si>
+    <t>Amphiroa</t>
+  </si>
+  <si>
+    <t>Tunicata</t>
+  </si>
+  <si>
+    <t>Historic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -152,7 +175,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,14 +486,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D09B8D9-703C-0142-BD23-9C6200179301}">
-  <dimension ref="A1:G55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="133" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
@@ -479,7 +502,7 @@
     <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>6</v>
       </c>
@@ -525,7 +548,7 @@
         <v>1.877</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>6</v>
       </c>
@@ -548,7 +571,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
@@ -571,7 +594,7 @@
         <v>0.68899999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
@@ -594,7 +617,7 @@
         <v>1.7330000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -617,7 +640,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9</v>
       </c>
@@ -640,7 +663,7 @@
         <v>2.2679999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9</v>
       </c>
@@ -663,7 +686,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -686,7 +709,7 @@
         <v>2.9990000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -709,7 +732,7 @@
         <v>0.74399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -732,7 +755,7 @@
         <v>1.165</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
@@ -755,7 +778,7 @@
         <v>2.4449999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>13</v>
       </c>
@@ -778,7 +801,7 @@
         <v>1.712</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -801,7 +824,7 @@
         <v>1.224</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>18</v>
       </c>
@@ -824,7 +847,7 @@
         <v>0.92800000000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>18</v>
       </c>
@@ -847,7 +870,7 @@
         <v>2.4780000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>18</v>
       </c>
@@ -870,7 +893,7 @@
         <v>2.1989999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
@@ -893,7 +916,7 @@
         <v>1.845</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5</v>
       </c>
@@ -916,7 +939,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>5</v>
       </c>
@@ -939,7 +962,7 @@
         <v>2.1150000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -962,7 +985,7 @@
         <v>1.839</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -985,7 +1008,7 @@
         <v>1.8979999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1008,7 +1031,7 @@
         <v>0.64700000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1031,7 +1054,7 @@
         <v>3.085</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>10</v>
       </c>
@@ -1054,7 +1077,7 @@
         <v>4.6360000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1077,7 +1100,7 @@
         <v>25.646999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1100,7 +1123,7 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1123,7 +1146,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1146,7 +1169,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1169,7 +1192,7 @@
         <v>26.469000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1192,7 +1215,7 @@
         <v>8.0449999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1215,7 +1238,7 @@
         <v>1.7989999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1238,7 +1261,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1261,7 +1284,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1284,7 +1307,7 @@
         <v>141.691</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1307,7 +1330,7 @@
         <v>159.30699999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1330,7 +1353,7 @@
         <v>2.8809999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1353,7 +1376,7 @@
         <v>142.90600000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1376,7 +1399,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>19</v>
       </c>
@@ -1399,7 +1422,7 @@
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>19</v>
       </c>
@@ -1422,7 +1445,7 @@
         <v>1.508</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>19</v>
       </c>
@@ -1445,7 +1468,7 @@
         <v>1.2410000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>19</v>
       </c>
@@ -1468,7 +1491,7 @@
         <v>53.000999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>19</v>
       </c>
@@ -1491,7 +1514,7 @@
         <v>58.883000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>11</v>
       </c>
@@ -1514,7 +1537,7 @@
         <v>70.054000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>11</v>
       </c>
@@ -1537,7 +1560,7 @@
         <v>2.2559999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>11</v>
       </c>
@@ -1560,7 +1583,7 @@
         <v>0.92900000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>11</v>
       </c>
@@ -1583,7 +1606,7 @@
         <v>154.74</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>29</v>
       </c>
@@ -1606,7 +1629,7 @@
         <v>14.69</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>29</v>
       </c>
@@ -1629,7 +1652,7 @@
         <v>1.8120000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>29</v>
       </c>
@@ -1652,7 +1675,7 @@
         <v>1.2949999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>29</v>
       </c>
@@ -1675,7 +1698,7 @@
         <v>116.37</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>29</v>
       </c>
@@ -1698,7 +1721,7 @@
         <v>0.46600000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>14</v>
       </c>
@@ -1708,8 +1731,20 @@
       <c r="C54" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1">
+        <v>44.261000000000003</v>
+      </c>
+      <c r="F54" s="1">
+        <v>136.459</v>
+      </c>
+      <c r="G54" s="1">
+        <v>98.796999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>14</v>
       </c>
@@ -1718,6 +1753,726 @@
       </c>
       <c r="C55" t="s">
         <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0.502</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1.3089999999999999</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.629</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F56" s="1">
+        <v>15.154</v>
+      </c>
+      <c r="G56" s="1">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="F57" s="1">
+        <v>4.5620000000000003</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="1">
+        <v>97.47</v>
+      </c>
+      <c r="F58" s="1">
+        <v>134.369</v>
+      </c>
+      <c r="G58" s="1">
+        <v>114.759</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.377</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1.143</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0.59899999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="F61" s="1">
+        <v>2.488</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="1">
+        <v>45.618000000000002</v>
+      </c>
+      <c r="F63" s="1">
+        <v>103.602</v>
+      </c>
+      <c r="G63" s="1">
+        <v>69.254000000000005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0.73</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0.71099999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>28</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>28</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>28</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>28</v>
+      </c>
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>28</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>8</v>
+      </c>
+      <c r="B78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>8</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>8</v>
+      </c>
+      <c r="B83" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>8</v>
+      </c>
+      <c r="B84" t="s">
+        <v>24</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>8</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>8</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>7</v>
+      </c>
+      <c r="B88" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>7</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>7</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>7</v>
+      </c>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>7</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95" t="s">
+        <v>24</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>4</v>
+      </c>
+      <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>4</v>
+      </c>
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>4</v>
+      </c>
+      <c r="B99" t="s">
+        <v>24</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>24</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>